<commit_message>
paso: change ocrtxt value
</commit_message>
<xml_diff>
--- a/src/test/resources/datafiles/Cambio_Pantalla_Final_HyO_insumo_ConPagos.xlsx
+++ b/src/test/resources/datafiles/Cambio_Pantalla_Final_HyO_insumo_ConPagos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cfroc\Documents\trabajo 2021\grupo HDI\Trabajo Bancolombia\Framework SBDD\autoStarc\HDISerenityStarc\src\test\resources\datafiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos HDI BanColombia\HDISerenityStarc\HDISerenityStarc\src\test\resources\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EC41C0-63F2-4528-941E-47962516291A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE66A236-C8DE-4A63-BB8C-BF61A0AE755B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{41ECAC2F-6418-456A-8F01-BA8343D43682}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{41ECAC2F-6418-456A-8F01-BA8343D43682}"/>
   </bookViews>
   <sheets>
     <sheet name="dataConPagos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="270">
   <si>
     <t>ESCENARIO</t>
   </si>
@@ -1239,17 +1239,17 @@
   <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="7"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>137</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>268</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>269</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>138</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>139</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>140</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>141</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>142</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>143</v>
       </c>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>144</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>145</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>146</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>147</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>148</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>149</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>150</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>151</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>152</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>153</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>154</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>155</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>156</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>157</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>158</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>159</v>
       </c>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>160</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>161</v>
       </c>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>162</v>
       </c>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>163</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>164</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>165</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>166</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>167</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>168</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>169</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>170</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>171</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>172</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>173</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>174</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>175</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>176</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>177</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>178</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>179</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>180</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>181</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>182</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>183</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>184</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>185</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>186</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>187</v>
       </c>
@@ -1973,7 +1973,7 @@
       </c>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>188</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>189</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>190</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>191</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>192</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>193</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>194</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>195</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>196</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>197</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>198</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>199</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>200</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>201</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>202</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>203</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>204</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>205</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>206</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>207</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>208</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>209</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>210</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>211</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>212</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>213</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>214</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>215</v>
       </c>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="D81" s="6"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>216</v>
       </c>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>217</v>
       </c>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>218</v>
       </c>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>219</v>
       </c>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>220</v>
       </c>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>221</v>
       </c>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>222</v>
       </c>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>223</v>
       </c>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>224</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>225</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>226</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>227</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>228</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>229</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>230</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>231</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>232</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>233</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>234</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>235</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>236</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>237</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>238</v>
       </c>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="D104" s="6"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>239</v>
       </c>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="D105" s="6"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>240</v>
       </c>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="D106" s="6"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>241</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>242</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>243</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>244</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="D110" s="6"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>245</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>246</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>247</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>248</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>249</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>250</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>251</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>252</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>253</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>254</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>255</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>256</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>257</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>258</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>259</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>260</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>261</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>262</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>263</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>264</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="D130" s="6"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>265</v>
       </c>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="D131" s="6"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>266</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>267</v>
       </c>
@@ -3071,15 +3071,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADF81D9-EC70-402A-A1C1-81434612B3EE}">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>137</v>
       </c>
@@ -3093,7 +3096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>268</v>
       </c>
@@ -3107,415 +3110,386 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="6">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finalizada para cambios de retirar recibo
</commit_message>
<xml_diff>
--- a/src/test/resources/datafiles/Cambio_Pantalla_Final_HyO_insumo_ConPagos.xlsx
+++ b/src/test/resources/datafiles/Cambio_Pantalla_Final_HyO_insumo_ConPagos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos HDI BanColombia\HDISerenityStarc\HDISerenityStarc\src\test\resources\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE66A236-C8DE-4A63-BB8C-BF61A0AE755B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156EAFAD-80EF-4249-BC5D-ECCD8ED8D89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{41ECAC2F-6418-456A-8F01-BA8343D43682}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{41ECAC2F-6418-456A-8F01-BA8343D43682}"/>
   </bookViews>
   <sheets>
     <sheet name="dataConPagos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="271">
   <si>
     <t>ESCENARIO</t>
   </si>
@@ -849,6 +849,9 @@
   </si>
   <si>
     <t>object:33</t>
+  </si>
+  <si>
+    <t>65</t>
   </si>
 </sst>
 </file>
@@ -1238,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7142A162-F17C-443F-9FA3-2F3CFA290558}">
   <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D2" s="6">
         <v>385</v>
@@ -1285,7 +1288,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D3" s="6">
         <v>385</v>
@@ -1299,7 +1302,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D4" s="6">
         <v>385</v>
@@ -1313,7 +1316,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D5" s="6">
         <v>385</v>
@@ -1327,7 +1330,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D6" s="6">
         <v>385</v>
@@ -1341,7 +1344,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6">
         <v>385</v>
@@ -1355,7 +1358,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D8" s="6">
         <v>385</v>
@@ -1381,7 +1384,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D10" s="6">
         <v>385</v>
@@ -1395,7 +1398,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D11" s="6">
         <v>385</v>
@@ -1421,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D13" s="6">
         <v>385</v>
@@ -1435,7 +1438,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D14" s="6">
         <v>385</v>
@@ -1449,7 +1452,7 @@
         <v>17</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D15" s="6">
         <v>385</v>
@@ -1463,7 +1466,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D16" s="6">
         <v>385</v>
@@ -1477,7 +1480,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D17" s="6">
         <v>385</v>
@@ -1491,7 +1494,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D18" s="6">
         <v>385</v>
@@ -1505,7 +1508,7 @@
         <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D19" s="6">
         <v>385</v>
@@ -1519,7 +1522,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D20" s="6">
         <v>385</v>
@@ -1533,7 +1536,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D21" s="6">
         <v>385</v>
@@ -1547,7 +1550,7 @@
         <v>24</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D22" s="6">
         <v>385</v>
@@ -1561,7 +1564,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D23" s="6">
         <v>385</v>
@@ -1635,7 +1638,7 @@
         <v>31</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D29" s="6">
         <v>385</v>
@@ -1649,7 +1652,7 @@
         <v>32</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D30" s="6">
         <v>385</v>
@@ -1663,7 +1666,7 @@
         <v>33</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D31" s="6">
         <v>385</v>
@@ -1677,7 +1680,7 @@
         <v>34</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D32" s="6">
         <v>385</v>
@@ -1691,7 +1694,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D33" s="6">
         <v>385</v>
@@ -1705,7 +1708,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D34" s="6">
         <v>385</v>
@@ -1719,7 +1722,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D35" s="6">
         <v>385</v>
@@ -1733,7 +1736,7 @@
         <v>38</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D36" s="6">
         <v>385</v>
@@ -1747,7 +1750,7 @@
         <v>39</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D37" s="6">
         <v>385</v>
@@ -1761,7 +1764,7 @@
         <v>40</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D38" s="6">
         <v>385</v>
@@ -1787,7 +1790,7 @@
         <v>42</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D40" s="6">
         <v>385</v>
@@ -1801,7 +1804,7 @@
         <v>43</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D41" s="6">
         <v>385</v>
@@ -1815,7 +1818,7 @@
         <v>44</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D42" s="6">
         <v>385</v>
@@ -1829,7 +1832,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D43" s="6">
         <v>385</v>
@@ -1843,7 +1846,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D44" s="6">
         <v>385</v>
@@ -1857,7 +1860,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D45" s="6">
         <v>385</v>
@@ -1871,7 +1874,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D46" s="6">
         <v>385</v>
@@ -1885,7 +1888,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D47" s="6">
         <v>385</v>
@@ -1899,7 +1902,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D48" s="6">
         <v>385</v>
@@ -1913,7 +1916,7 @@
         <v>51</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D49" s="6">
         <v>385</v>
@@ -1927,7 +1930,7 @@
         <v>52</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D50" s="6">
         <v>385</v>
@@ -1941,7 +1944,7 @@
         <v>53</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D51" s="6">
         <v>385</v>
@@ -1955,7 +1958,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D52" s="6">
         <v>385</v>
@@ -1993,7 +1996,7 @@
         <v>57</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D55" s="6">
         <v>385</v>
@@ -2007,7 +2010,7 @@
         <v>58</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D56" s="6">
         <v>385</v>
@@ -2021,7 +2024,7 @@
         <v>59</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D57" s="6">
         <v>385</v>
@@ -2035,7 +2038,7 @@
         <v>60</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D58" s="6">
         <v>385</v>
@@ -2049,7 +2052,7 @@
         <v>61</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D59" s="6">
         <v>385</v>
@@ -2063,7 +2066,7 @@
         <v>62</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D60" s="6">
         <v>385</v>
@@ -2077,7 +2080,7 @@
         <v>63</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D61" s="6">
         <v>385</v>
@@ -2091,7 +2094,7 @@
         <v>64</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D62" s="6">
         <v>385</v>
@@ -2105,7 +2108,7 @@
         <v>65</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D63" s="6">
         <v>385</v>
@@ -2119,7 +2122,7 @@
         <v>66</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D64" s="6">
         <v>385</v>
@@ -2133,7 +2136,7 @@
         <v>67</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D65" s="6">
         <v>385</v>
@@ -2147,7 +2150,7 @@
         <v>68</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D66" s="6">
         <v>385</v>
@@ -2161,7 +2164,7 @@
         <v>69</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D67" s="6">
         <v>385</v>
@@ -2175,7 +2178,7 @@
         <v>70</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D68" s="6">
         <v>385</v>
@@ -2189,7 +2192,7 @@
         <v>71</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D69" s="6">
         <v>385</v>
@@ -2203,7 +2206,7 @@
         <v>72</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D70" s="6">
         <v>385</v>
@@ -2217,7 +2220,7 @@
         <v>73</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D71" s="6">
         <v>385</v>
@@ -2231,7 +2234,7 @@
         <v>74</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D72" s="6">
         <v>385</v>
@@ -2245,7 +2248,7 @@
         <v>75</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D73" s="6">
         <v>385</v>
@@ -2259,7 +2262,7 @@
         <v>76</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D74" s="6">
         <v>385</v>
@@ -2273,7 +2276,7 @@
         <v>77</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D75" s="6">
         <v>385</v>
@@ -2287,7 +2290,7 @@
         <v>78</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D76" s="6">
         <v>385</v>
@@ -2301,7 +2304,7 @@
         <v>79</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D77" s="6">
         <v>385</v>
@@ -2315,7 +2318,7 @@
         <v>80</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D78" s="6">
         <v>385</v>
@@ -2329,7 +2332,7 @@
         <v>81</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D79" s="6">
         <v>385</v>
@@ -2343,7 +2346,7 @@
         <v>82</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D80" s="6">
         <v>385</v>
@@ -2465,7 +2468,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D90" s="6">
         <v>385</v>
@@ -2479,7 +2482,7 @@
         <v>93</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D91" s="6">
         <v>385</v>
@@ -2493,7 +2496,7 @@
         <v>94</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D92" s="6">
         <v>385</v>
@@ -2507,7 +2510,7 @@
         <v>95</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D93" s="6">
         <v>385</v>
@@ -2521,7 +2524,7 @@
         <v>96</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D94" s="6">
         <v>385</v>
@@ -2535,7 +2538,7 @@
         <v>97</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D95" s="6">
         <v>385</v>
@@ -2549,7 +2552,7 @@
         <v>98</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D96" s="6">
         <v>385</v>
@@ -2563,7 +2566,7 @@
         <v>99</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D97" s="6">
         <v>385</v>
@@ -2577,7 +2580,7 @@
         <v>100</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D98" s="6">
         <v>385</v>
@@ -2591,7 +2594,7 @@
         <v>101</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D99" s="6">
         <v>385</v>
@@ -2605,7 +2608,7 @@
         <v>102</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D100" s="6">
         <v>385</v>
@@ -2619,7 +2622,7 @@
         <v>103</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="D101" s="6">
         <v>385</v>
@@ -2877,10 +2880,10 @@
         <v>122</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D120" s="6">
-        <v>385</v>
+        <v>3</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2891,10 +2894,10 @@
         <v>123</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D121" s="6">
-        <v>385</v>
+        <v>3</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2905,10 +2908,10 @@
         <v>124</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D122" s="6">
-        <v>385</v>
+        <v>3</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2919,10 +2922,10 @@
         <v>125</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D123" s="6">
-        <v>385</v>
+        <v>3</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3066,6 +3069,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D120:D123" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3073,7 +3079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADF81D9-EC70-402A-A1C1-81434612B3EE}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>